<commit_message>
Updated backend, frontend pages and email template
</commit_message>
<xml_diff>
--- a/SmartRecruit-main/backend/data/67b98bc79dec34f62a72c1d9.xlsx
+++ b/SmartRecruit-main/backend/data/67b98bc79dec34f62a72c1d9.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anjal\OneDrive\Desktop\final\SmartRecruit\SmartRecruit-main\backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F794BA-2132-4633-9943-9CA526D307D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C828DCEE-05A4-4BE2-BC81-E51EBE37135D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,12 +31,6 @@
     <t>Score</t>
   </si>
   <si>
-    <t xml:space="preserve">Dhanush </t>
-  </si>
-  <si>
-    <t>bro</t>
-  </si>
-  <si>
     <t>kaniz.zc@gmail.com</t>
   </si>
   <si>
@@ -53,6 +47,12 @@
   </si>
   <si>
     <t>19p0031@gmail.com</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>asmi</t>
   </si>
 </sst>
 </file>
@@ -440,13 +440,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -461,10 +464,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>95</v>
@@ -472,10 +475,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>80</v>
@@ -483,10 +486,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>65</v>
@@ -494,13 +497,19 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="C6">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -512,7 +521,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:C1 A4 C2 C3 A5 C5 C4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C1 C2 C3 C5 C4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>